<commit_message>
Provato ad inserire configurazione a scelta per la sequenza delle ricerche locali; rimane fallace
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/errori_lettura.xlsx
+++ b/PS-VRP/Dati_output/errori_lettura.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P99"/>
+  <dimension ref="A1:P109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,7 +552,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>243335</v>
+        <v>235572</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>243569</v>
+        <v>243335</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>244023</v>
+        <v>243569</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -597,12 +597,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>245623</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>244023</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -617,7 +612,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>245089</v>
+        <v>245623</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -636,33 +631,33 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>250284</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A8" t="n">
+        <v>250759</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>251500</v>
+      <c r="A9" s="1" t="n">
+        <v>245090</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>251519</v>
+        <v>245089</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -681,105 +676,145 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>251070</v>
+      <c r="A11" s="1" t="n">
+        <v>251109</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>251631</v>
+      <c r="A12" s="1" t="n">
+        <v>250284</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>251310</v>
+        <v>251211</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>251237</v>
+      <c r="A14" s="1" t="n">
+        <v>251346</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>252084</v>
+      <c r="A15" s="1" t="n">
+        <v>251519</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251752</v>
+        <v>250923</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>251573</v>
+      <c r="A17" s="1" t="n">
+        <v>251044</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>251362</v>
+      <c r="A18" s="1" t="n">
+        <v>250591</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>251410</v>
-      </c>
-      <c r="I19" t="inlineStr">
+        <v>245275</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>252109</v>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A20" t="n">
+        <v>251050</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>251186</v>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A21" t="n">
+        <v>251227</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>251895</v>
-      </c>
-      <c r="H22" t="inlineStr">
+        <v>251005</v>
+      </c>
+      <c r="L22" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -787,34 +822,49 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>251897</v>
-      </c>
-      <c r="H23" t="inlineStr">
+        <v>250918</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>251655</v>
+      <c r="A24" s="1" t="n">
+        <v>251310</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>251905</v>
+        <v>251081</v>
       </c>
       <c r="H25" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -822,42 +872,97 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>252235</v>
+        <v>251080</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>251082</v>
+      <c r="A27" s="1" t="n">
+        <v>251079</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>251218</v>
+      <c r="A28" s="1" t="n">
+        <v>251078</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>251219</v>
+      <c r="A29" s="1" t="n">
+        <v>250819</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>252107</v>
+        <v>251247</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -871,48 +976,38 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>251792</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A31" t="n">
+        <v>251225</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>251972</v>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A32" t="n">
+        <v>251421</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>251565</v>
+        <v>251268</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>252081</v>
+      <c r="A34" s="1" t="n">
+        <v>244960</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>251180</v>
+        <v>251371</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -921,198 +1016,118 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>251780</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A36" t="n">
+        <v>251782</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>252112</v>
+      <c r="A37" s="1" t="n">
+        <v>250913</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>251773</v>
+      <c r="A38" s="1" t="n">
+        <v>251846</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>252111</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A39" t="n">
+        <v>251477</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>252025</v>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A40" t="n">
+        <v>251054</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>252058</v>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A41" t="n">
+        <v>251396</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>251944</v>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A42" t="n">
+        <v>251453</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>252337</v>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A43" t="n">
+        <v>251455</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>251612</v>
+        <v>251391</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>252282</v>
+      <c r="A45" s="1" t="n">
+        <v>251651</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>251879</v>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A46" t="n">
+        <v>251840</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>252108</v>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A47" t="n">
+        <v>251548</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>251916</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A48" t="n">
+        <v>251547</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>251911</v>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A49" t="n">
+        <v>251742</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>251454</v>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A50" t="n">
+        <v>251395</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>252196</v>
+        <v>251466</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -1127,7 +1142,12 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>252156</v>
+        <v>251750</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -1141,28 +1161,18 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>252258</v>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A53" t="n">
+        <v>251456</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>251762</v>
+        <v>251340</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -1177,12 +1187,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>251943</v>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251283</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -1197,7 +1202,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>251445</v>
+        <v>251245</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -1212,7 +1217,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>251910</v>
+        <v>251061</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -1227,7 +1232,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>251992</v>
+        <v>251062</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -1242,12 +1247,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>252279</v>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251246</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -1262,19 +1262,14 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>251985</v>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
+        <v>245350</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1282,24 +1277,14 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>251984</v>
+        <v>251164</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>251763</v>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
+        <v>250874</v>
+      </c>
+      <c r="L62" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1307,19 +1292,9 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>251890</v>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P63" t="inlineStr">
+        <v>251257</v>
+      </c>
+      <c r="L63" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1327,19 +1302,9 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>251287</v>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
+        <v>251229</v>
+      </c>
+      <c r="H64" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1347,7 +1312,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>251772</v>
+        <v>251463</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -1362,7 +1327,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>252195</v>
+        <v>251580</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -1377,7 +1342,17 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>251741</v>
+        <v>251650</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -1392,7 +1367,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>251935</v>
+        <v>251416</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -1407,12 +1382,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>251677</v>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>250641</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -1427,12 +1397,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>252229</v>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251464</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -1447,7 +1412,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>252375</v>
+        <v>251465</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -1462,7 +1427,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>252395</v>
+        <v>251462</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -1477,7 +1442,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>252410</v>
+        <v>251467</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -1492,7 +1457,12 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>252325</v>
+        <v>251795</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -1506,23 +1476,13 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>252326</v>
-      </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P75" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A75" t="n">
+        <v>251284</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>251680</v>
+        <v>251520</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -1537,7 +1497,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>251679</v>
+        <v>251987</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -1552,7 +1512,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>251684</v>
+        <v>251374</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -1567,12 +1527,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>252228</v>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>250894</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -1587,7 +1542,12 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>251798</v>
+        <v>251746</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -1602,7 +1562,17 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>252110</v>
+        <v>251585</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -1617,7 +1587,12 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>252121</v>
+        <v>251260</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -1632,7 +1607,12 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>251978</v>
+        <v>251373</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -1647,7 +1627,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>251993</v>
+        <v>244354</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
@@ -1667,7 +1647,12 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>251747</v>
+        <v>244355</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -1682,7 +1667,12 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>251917</v>
+        <v>251594</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -1697,7 +1687,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>251390</v>
+        <v>251743</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
@@ -1717,19 +1707,9 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>251901</v>
+        <v>251424</v>
       </c>
       <c r="H88" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1747,9 +1727,9 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>251479</v>
-      </c>
-      <c r="I89" t="inlineStr">
+        <v>251397</v>
+      </c>
+      <c r="H89" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1767,7 +1747,12 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>251681</v>
+        <v>244204</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -1782,9 +1767,9 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>251717</v>
-      </c>
-      <c r="I91" t="inlineStr">
+        <v>251561</v>
+      </c>
+      <c r="H91" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1802,7 +1787,12 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>252293</v>
+        <v>251564</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O92" t="inlineStr">
         <is>
@@ -1817,7 +1807,12 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>251979</v>
+        <v>251809</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -1832,7 +1827,12 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>251898</v>
+        <v>251566</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O94" t="inlineStr">
         <is>
@@ -1847,12 +1847,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>251958</v>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251626</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -1867,9 +1862,9 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>250914</v>
-      </c>
-      <c r="L96" t="inlineStr">
+        <v>251475</v>
+      </c>
+      <c r="H96" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1887,7 +1882,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>252042</v>
+        <v>251761</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -1902,7 +1897,17 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>252082</v>
+        <v>251502</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -1917,24 +1922,159 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>252290</v>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P99" t="inlineStr">
+        <v>251706</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>251505</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>251557</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P101" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>251562</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>251546</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P103" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>250670</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>251485</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>251259</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>251252</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>251249</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>251251</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>

</xml_diff>

<commit_message>
Versione finale (direi) per ISTITUTO STAMPA
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/errori_lettura.xlsx
+++ b/PS-VRP/Dati_output/errori_lettura.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P99"/>
+  <dimension ref="A1:P109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,7 +552,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>243335</v>
+        <v>235572</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>243569</v>
+        <v>243335</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>244023</v>
+        <v>243569</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -597,12 +597,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>245623</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>244023</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -617,7 +612,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>245089</v>
+        <v>245623</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -636,33 +631,33 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>250284</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A8" t="n">
+        <v>250759</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>251500</v>
+      <c r="A9" s="1" t="n">
+        <v>245090</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>251519</v>
+        <v>245089</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -681,105 +676,145 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>251070</v>
+      <c r="A11" s="1" t="n">
+        <v>251109</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>251631</v>
+      <c r="A12" s="1" t="n">
+        <v>250284</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>251310</v>
+        <v>251211</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>251237</v>
+      <c r="A14" s="1" t="n">
+        <v>251346</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>252084</v>
+      <c r="A15" s="1" t="n">
+        <v>251519</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251752</v>
+        <v>250923</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>251573</v>
+      <c r="A17" s="1" t="n">
+        <v>251044</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>251362</v>
+      <c r="A18" s="1" t="n">
+        <v>250591</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>251410</v>
-      </c>
-      <c r="I19" t="inlineStr">
+        <v>245275</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>252109</v>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A20" t="n">
+        <v>251050</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>251186</v>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A21" t="n">
+        <v>251227</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>251895</v>
-      </c>
-      <c r="H22" t="inlineStr">
+        <v>251005</v>
+      </c>
+      <c r="L22" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -787,34 +822,49 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>251897</v>
-      </c>
-      <c r="H23" t="inlineStr">
+        <v>250918</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>251655</v>
+      <c r="A24" s="1" t="n">
+        <v>251310</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>251905</v>
+        <v>251081</v>
       </c>
       <c r="H25" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -822,42 +872,97 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>252235</v>
+        <v>251080</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>251082</v>
+      <c r="A27" s="1" t="n">
+        <v>251079</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>251218</v>
+      <c r="A28" s="1" t="n">
+        <v>251078</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>251219</v>
+      <c r="A29" s="1" t="n">
+        <v>250819</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>252107</v>
+        <v>251247</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -871,48 +976,38 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>251792</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A31" t="n">
+        <v>251225</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>251972</v>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A32" t="n">
+        <v>251421</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>251565</v>
+        <v>251268</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>252081</v>
+      <c r="A34" s="1" t="n">
+        <v>244960</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>251180</v>
+        <v>251371</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -921,198 +1016,118 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>251780</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A36" t="n">
+        <v>251782</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>252112</v>
+      <c r="A37" s="1" t="n">
+        <v>250913</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>251773</v>
+      <c r="A38" s="1" t="n">
+        <v>251846</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>252111</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A39" t="n">
+        <v>251477</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>252025</v>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A40" t="n">
+        <v>251054</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>252058</v>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A41" t="n">
+        <v>251396</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>251944</v>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A42" t="n">
+        <v>251453</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>252337</v>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A43" t="n">
+        <v>251455</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>251612</v>
+        <v>251391</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>252282</v>
+      <c r="A45" s="1" t="n">
+        <v>251651</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>251879</v>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A46" t="n">
+        <v>251840</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>252108</v>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A47" t="n">
+        <v>251548</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>251916</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A48" t="n">
+        <v>251547</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>251911</v>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A49" t="n">
+        <v>251742</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>251454</v>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A50" t="n">
+        <v>251395</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>252196</v>
+        <v>251466</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -1127,7 +1142,12 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>252156</v>
+        <v>251750</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -1141,28 +1161,18 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>252258</v>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A53" t="n">
+        <v>251456</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>251762</v>
+        <v>251340</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -1177,12 +1187,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>251943</v>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251283</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -1197,7 +1202,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>251445</v>
+        <v>251245</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -1212,7 +1217,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>251910</v>
+        <v>251061</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -1227,7 +1232,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>251992</v>
+        <v>251062</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -1242,12 +1247,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>252279</v>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251246</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -1262,19 +1262,14 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>251985</v>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
+        <v>245350</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1282,24 +1277,14 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>251984</v>
+        <v>251164</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>251763</v>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
+        <v>250874</v>
+      </c>
+      <c r="L62" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1307,19 +1292,9 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>251890</v>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P63" t="inlineStr">
+        <v>251257</v>
+      </c>
+      <c r="L63" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1327,19 +1302,9 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>251287</v>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
+        <v>251229</v>
+      </c>
+      <c r="H64" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1347,7 +1312,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>251772</v>
+        <v>251463</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -1362,7 +1327,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>252195</v>
+        <v>251580</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -1377,7 +1342,17 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>251741</v>
+        <v>251650</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -1392,7 +1367,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>251935</v>
+        <v>251416</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -1407,12 +1382,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>251677</v>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>250641</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -1427,12 +1397,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>252229</v>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251464</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -1447,7 +1412,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>252375</v>
+        <v>251465</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -1462,7 +1427,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>252395</v>
+        <v>251462</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -1477,7 +1442,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>252410</v>
+        <v>251467</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -1492,7 +1457,12 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>252325</v>
+        <v>251795</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -1506,23 +1476,13 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>252326</v>
-      </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P75" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A75" t="n">
+        <v>251284</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>251680</v>
+        <v>251520</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -1537,7 +1497,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>251679</v>
+        <v>251987</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -1552,7 +1512,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>251684</v>
+        <v>251374</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -1567,12 +1527,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>252228</v>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>250894</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -1587,7 +1542,12 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>251798</v>
+        <v>251746</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -1602,7 +1562,17 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>252110</v>
+        <v>251585</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -1617,7 +1587,12 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>252121</v>
+        <v>251260</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -1632,7 +1607,12 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>251978</v>
+        <v>251373</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -1647,7 +1627,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>251993</v>
+        <v>244354</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
@@ -1667,7 +1647,12 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>251747</v>
+        <v>244355</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -1682,7 +1667,12 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>251917</v>
+        <v>251594</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -1697,7 +1687,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>251390</v>
+        <v>251743</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
@@ -1717,19 +1707,9 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>251901</v>
+        <v>251424</v>
       </c>
       <c r="H88" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1747,9 +1727,9 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>251479</v>
-      </c>
-      <c r="I89" t="inlineStr">
+        <v>251397</v>
+      </c>
+      <c r="H89" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1767,7 +1747,12 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>251681</v>
+        <v>244204</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -1782,9 +1767,9 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>251717</v>
-      </c>
-      <c r="I91" t="inlineStr">
+        <v>251561</v>
+      </c>
+      <c r="H91" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1802,7 +1787,12 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>252293</v>
+        <v>251564</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O92" t="inlineStr">
         <is>
@@ -1817,7 +1807,12 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>251979</v>
+        <v>251809</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -1832,7 +1827,12 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>251898</v>
+        <v>251566</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O94" t="inlineStr">
         <is>
@@ -1847,12 +1847,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>251958</v>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251626</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -1867,9 +1862,9 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>250914</v>
-      </c>
-      <c r="L96" t="inlineStr">
+        <v>251475</v>
+      </c>
+      <c r="H96" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1887,7 +1882,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>252042</v>
+        <v>251761</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -1902,7 +1897,17 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>252082</v>
+        <v>251502</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -1917,24 +1922,159 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>252290</v>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P99" t="inlineStr">
+        <v>251706</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>251505</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>251557</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P101" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>251562</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>251546</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P103" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>250670</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>251485</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>251259</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>251252</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>251249</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>251251</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>

</xml_diff>

<commit_message>
Reso pathing compatibile anche con uso esterno a GitHub; implementata graficazione alternativa; Rimossi print output di testing e lasciato solo quello finale; Cambiati "fascia" e "fascia utile" da maiuscolo a minuscolo (forma attuale)
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/errori_lettura.xlsx
+++ b/PS-VRP/Dati_output/errori_lettura.xlsx
@@ -491,12 +491,12 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Commesse::FASCIA</t>
+          <t>Commesse::fascia</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Commesse::FASCIA UTILE</t>
+          <t>Commesse::fascia utile</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">

</xml_diff>